<commit_message>
Added image urls for all non-buffet items
</commit_message>
<xml_diff>
--- a/prototype/src/assets/items.xlsx
+++ b/prototype/src/assets/items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mythi\Desktop\cs4249_code\hc-experiment-prototypes\prototype\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73CD1D8-577A-4B40-8FB7-A09F2761497A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CBBEAC-DBF9-431F-ABFC-975C4B8512E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="items2" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="79">
   <si>
     <t>Category</t>
   </si>
@@ -178,6 +178,96 @@
   </si>
   <si>
     <t>Sold Out</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/81b281_e73279e3a2b04896801e9a4a596f2ef5~mv2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/81b281_d11fcee9f450476db2426a3994c5ff65~mv2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/81b281_bb0d5633862f4561850bf7189a5d4898~mv2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/81b281_5f3b07f7191049da86fe35649bec3576~mv2.jpeg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpeg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/81b281_11382e1a4c8741fbaeb8fa3358c5c3d7~mv2.jpeg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpeg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/81b281_9744daafc2a74c428e8e149e23157444~mv2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/81b281_3594c854f2b94d0db4aeaf471e622e80~mv2.png/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.png</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/81b281_0c3128c504504bc88d0a09d1637acfd0~mv2.png/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.png</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/81b281_a1cbbdb0cbb04264a7c2209887ef1de0~mv2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_675a1e6a0c8a4e59bea7b0c6fb87305c~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_f6929eeaeacf4768a4741fa92d3d0a13~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_a906145e41d344aa84b2ae5f7dc06bad~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_376010e315114512967b88f61ce5aac8~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_7fecede4a65e45c5b2be74d2f1f9a96a~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_c7e7e7da62fa421eb44a04d0a0a75212~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_d4e2d3567f3948bea2e372fd7d15e882~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_e3f680f508ca4fc99f472907fdaaa0e7~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_0613fcaa4a1244bf9e9f8eeb6fa13d5e~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_8fefc1a72dd547efa25f955ee9ed0739~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_ec4edc7c4767401fa2aca9c99c4b6435~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_31c6a3a69a16415580204587418a3f32~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_7a2184a79ff541abaf058a8cefd46c0c~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_047889907a0b4cb48c2c4e759ab53cda~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_645c098959444cab9aea93880a48588f~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_ea7be89998e845eaaf64de13e0ec60b6~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_8815774e5ffd4e3c94a4db02b99baa3f~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_466961d2b1674105b0bd8d6888f274e5~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_d2a0b64d63d64f24a4f2dad3bf009e06~mv2_d_3840_5760_s_4_2.jpeg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpeg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_644ba999acf24eeda80b46e46377bd57~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wixstatic.com/media/e7fc58_f6c67f87e38e4af0a9a59c36a0cae856~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
   </si>
 </sst>
 </file>
@@ -1031,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A34" sqref="A33:Q51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,7 +1180,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1106,8 +1196,8 @@
       <c r="D4">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
-        <v>8</v>
+      <c r="E4" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1124,7 +1214,7 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1141,7 +1231,7 @@
         <v>6.8</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1158,7 +1248,7 @@
         <v>6.8</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1175,7 +1265,7 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1192,7 +1282,7 @@
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1209,7 +1299,7 @@
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1226,7 +1316,7 @@
         <v>138</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1243,7 +1333,7 @@
         <v>1.6</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1260,7 +1350,7 @@
         <v>1.5</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1277,7 +1367,7 @@
         <v>1.6</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1294,7 +1384,7 @@
         <v>48</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1311,7 +1401,7 @@
         <v>1.6</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1328,7 +1418,7 @@
         <v>1.5</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1345,7 +1435,7 @@
         <v>1.7</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1362,7 +1452,7 @@
         <v>1.8</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1379,7 +1469,7 @@
         <v>1.8</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1396,7 +1486,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1413,7 +1503,7 @@
         <v>1.8</v>
       </c>
       <c r="E22" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1430,7 +1520,7 @@
         <v>1.8</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1447,7 +1537,7 @@
         <v>1.6</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1464,7 +1554,7 @@
         <v>1.8</v>
       </c>
       <c r="E25" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1481,7 +1571,7 @@
         <v>1.8</v>
       </c>
       <c r="E26" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1498,7 +1588,7 @@
         <v>1.8</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1515,7 +1605,7 @@
         <v>1.8</v>
       </c>
       <c r="E28" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1532,7 +1622,7 @@
         <v>1.8</v>
       </c>
       <c r="E29" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1549,7 +1639,7 @@
         <v>3.1</v>
       </c>
       <c r="E30" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1566,7 +1656,7 @@
         <v>1.5</v>
       </c>
       <c r="E31" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1583,12 +1673,13 @@
         <v>1.5</v>
       </c>
       <c r="E32" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{93475177-AF4A-41A7-8468-57CCF4B8D9C7}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{D275D903-9659-4194-8759-F5B0025C4312}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New trial task C. Fixed a few menu typoes.
</commit_message>
<xml_diff>
--- a/prototype/src/assets/items.xlsx
+++ b/prototype/src/assets/items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mythi\Desktop\cs4249_code\hc-experiment-prototypes\prototype\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CBBEAC-DBF9-431F-ABFC-975C4B8512E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E3E340-F1AD-4074-8815-1C99B6AE0171}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="items2" sheetId="1" r:id="rId1"/>
@@ -105,9 +105,6 @@
     <t>Set A: Stir-Fried Chicken Breast</t>
   </si>
   <si>
-    <t>Set B: Steamed Fish With Seawead Sauce</t>
-  </si>
-  <si>
     <t>Set A: Pandan Mock Chicken Mushroom Noodle</t>
   </si>
   <si>
@@ -132,12 +129,6 @@
     <t>Fishball OnStik</t>
   </si>
   <si>
-    <t>Soton Ball Onstik</t>
-  </si>
-  <si>
-    <t>Sotong Head Onstik</t>
-  </si>
-  <si>
     <t>Soton Wing OnStik</t>
   </si>
   <si>
@@ -268,6 +259,15 @@
   </si>
   <si>
     <t>https://static.wixstatic.com/media/e7fc58_f6c67f87e38e4af0a9a59c36a0cae856~mv2_d_3264_4896_s_4_2.jpg/v1/fill/w_466,h_350,usm_1.20_1.00_0.01/file.jpg</t>
+  </si>
+  <si>
+    <t>Soton Ball OnStik</t>
+  </si>
+  <si>
+    <t>Sotong Head OnStik</t>
+  </si>
+  <si>
+    <t>Set B: Steamed Fish With Seaweed Sauce</t>
   </si>
 </sst>
 </file>
@@ -1122,13 +1122,13 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" customWidth="1"/>
     <col min="3" max="3" width="37.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1180,7 +1180,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1197,7 +1197,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1214,7 +1214,7 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1231,7 +1231,7 @@
         <v>6.8</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1242,13 +1242,13 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="D7">
         <v>6.8</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1265,7 +1265,7 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1276,13 +1276,13 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9">
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1293,13 +1293,13 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10">
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1316,7 +1316,7 @@
         <v>138</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1327,13 +1327,13 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12">
         <v>1.6</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1344,13 +1344,13 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13">
         <v>1.5</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1361,13 +1361,13 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14">
         <v>1.6</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1378,13 +1378,13 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1395,13 +1395,13 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16">
         <v>1.6</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1412,13 +1412,13 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17">
         <v>1.5</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1429,13 +1429,13 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="D18">
         <v>1.7</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1446,13 +1446,13 @@
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="D19">
         <v>1.8</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1463,13 +1463,13 @@
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D20">
         <v>1.8</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1480,13 +1480,13 @@
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D21">
         <v>2.2000000000000002</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1497,13 +1497,13 @@
         <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D22">
         <v>1.8</v>
       </c>
       <c r="E22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1514,13 +1514,13 @@
         <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D23">
         <v>1.8</v>
       </c>
       <c r="E23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1531,13 +1531,13 @@
         <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D24">
         <v>1.6</v>
       </c>
       <c r="E24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1548,13 +1548,13 @@
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D25">
         <v>1.8</v>
       </c>
       <c r="E25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1565,13 +1565,13 @@
         <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D26">
         <v>1.8</v>
       </c>
       <c r="E26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1582,13 +1582,13 @@
         <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D27">
         <v>1.8</v>
       </c>
       <c r="E27" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1599,13 +1599,13 @@
         <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D28">
         <v>1.8</v>
       </c>
       <c r="E28" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1616,13 +1616,13 @@
         <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D29">
         <v>1.8</v>
       </c>
       <c r="E29" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1633,13 +1633,13 @@
         <v>17</v>
       </c>
       <c r="C30" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D30">
         <v>3.1</v>
       </c>
       <c r="E30" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1650,13 +1650,13 @@
         <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D31">
         <v>1.5</v>
       </c>
       <c r="E31" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1667,13 +1667,13 @@
         <v>18</v>
       </c>
       <c r="C32" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D32">
         <v>1.5</v>
       </c>
       <c r="E32" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>